<commit_message>
update: Fix metric inside function evaluate
</commit_message>
<xml_diff>
--- a/evaluators/dataset_column.xlsx
+++ b/evaluators/dataset_column.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pras\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\codes\nl2sql\evaluators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCDC4FCD-DE0E-4704-8282-C6E833B6E093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1FA4AC-8EFE-4E94-ACE4-2C596F76E2D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8A2B21AD-AFBD-4AFB-8E0A-24CCC2B22D2D}"/>
   </bookViews>
@@ -47,72 +47,36 @@
     <t>keterangan</t>
   </si>
   <si>
-    <t>Tampilkan semua data barang.</t>
-  </si>
-  <si>
     <t>*</t>
   </si>
   <si>
     <t>inventori_1.json</t>
   </si>
   <si>
-    <t>Tampilkan nama dan stok semua barang.</t>
-  </si>
-  <si>
     <t>nama_barang, stok</t>
   </si>
   <si>
-    <t>Tampilkan semua barang dengan stok kurang dari 10.</t>
-  </si>
-  <si>
-    <t>Tampilkan barang dengan harga lebih dari 100000.</t>
-  </si>
-  <si>
     <t>Tampilkan semua pemasok yang alamatnya di Jakarta.</t>
   </si>
   <si>
     <t>Tampilkan semua pembelian yang dilakukan oleh pemasok dengan ID 2.</t>
   </si>
   <si>
-    <t>Hitung jumlah total barang yang tersedia.</t>
-  </si>
-  <si>
     <t>stok</t>
   </si>
   <si>
-    <t>Tampilkan nama barang dan kategori dari semua barang.</t>
-  </si>
-  <si>
     <t>nama_barang, nama_kategori</t>
   </si>
   <si>
-    <t>Tampilkan semua barang yang termasuk dalam kategori “Elektronik”.</t>
-  </si>
-  <si>
-    <t>Tampilkan daftar barang yang pernah dibeli beserta jumlah yang dibeli.</t>
-  </si>
-  <si>
     <t>nama_barang, jumlah</t>
   </si>
   <si>
-    <t>Tampilkan tanggal dan tujuan dari semua pengeluaran barang.</t>
-  </si>
-  <si>
     <t>tanggal, tujuan</t>
   </si>
   <si>
-    <t>Tampilkan pengeluaran barang yang terjadi setelah tanggal 1 Januari 2024.</t>
-  </si>
-  <si>
-    <t>Hitung total pengeluaran barang (jumlah item keluar).</t>
-  </si>
-  <si>
     <t>jumlah</t>
   </si>
   <si>
-    <t>Tampilkan 5 barang dengan stok paling sedikit.</t>
-  </si>
-  <si>
     <t>Tampilkan nama pemasok dan tanggal pembelian untuk semua transaksi.</t>
   </si>
   <si>
@@ -123,6 +87,42 @@
   </si>
   <si>
     <t>kalimat</t>
+  </si>
+  <si>
+    <t>Tampilkan semua data produk.</t>
+  </si>
+  <si>
+    <t>Tampilkan nama dan stok semua produk.</t>
+  </si>
+  <si>
+    <t>Tampilkan semua produk dengan stok kurang dari 10.</t>
+  </si>
+  <si>
+    <t>Tampilkan produk dengan harga lebih dari 100000.</t>
+  </si>
+  <si>
+    <t>Hitung jumlah total produk yang tersedia.</t>
+  </si>
+  <si>
+    <t>Tampilkan nama produk dan kategori dari semua produk.</t>
+  </si>
+  <si>
+    <t>Tampilkan semua produk yang termasuk dalam kategori “Elektronik”.</t>
+  </si>
+  <si>
+    <t>Tampilkan daftar produk yang pernah dibeli beserta jumlah yang dibeli.</t>
+  </si>
+  <si>
+    <t>Tampilkan tanggal dan tujuan dari semua pengeluaran produk.</t>
+  </si>
+  <si>
+    <t>Tampilkan pengeluaran produk yang terjadi setelah tanggal 1 Januari 2024.</t>
+  </si>
+  <si>
+    <t>Hitung total pengeluaran produk (jumlah item keluar).</t>
+  </si>
+  <si>
+    <t>Tampilkan 5 produk dengan stok paling sedikit.</t>
   </si>
 </sst>
 </file>
@@ -194,7 +194,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,7 +532,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,10 +549,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -566,13 +566,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="3"/>
     </row>
@@ -581,13 +581,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -596,13 +596,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -611,13 +611,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -626,13 +626,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -641,13 +641,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -656,13 +656,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="3"/>
     </row>
@@ -671,13 +671,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -686,13 +686,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -701,13 +701,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -716,13 +716,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -731,13 +731,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -746,13 +746,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -761,13 +761,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E15" s="3"/>
     </row>
@@ -776,13 +776,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" s="3"/>
     </row>

</xml_diff>